<commit_message>
Added the results for benchmarks
</commit_message>
<xml_diff>
--- a/benchmark/micro/results.xlsx
+++ b/benchmark/micro/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lwyeluo/Workspaces/lab-project/browser/tim-evaluate/benchmark/micro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F556B2-9EB7-894A-87DA-76A83E24C1D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49785785-8D88-BC4C-9CC5-B7E70669E1E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{A38FA40B-9AA0-234E-B7A1-9A1E5346C45F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
   <si>
     <t>recordTask</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>updateFrameChain</t>
+  </si>
+  <si>
+    <t>CPU cycle</t>
   </si>
 </sst>
 </file>
@@ -135,7 +138,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>cpu cycle</c:v>
+                  <c:v>CPU cycle</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -160,10 +163,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'micro-benchmark'!$A$6:$A$98</c:f>
+              <c:f>'micro-benchmark'!$A$6:$A$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="93"/>
+                <c:ptCount val="78"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -300,147 +303,102 @@
                   <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>47</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>49</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>51</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>52</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>54</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>55</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>56</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>58</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>59</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>60</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>61</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>62</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>63</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>64</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>65</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>66</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>67</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>68</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>69</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>70</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>71</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>73</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>74</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>75</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>76</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>77</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>78</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>79</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>80</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>81</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>82</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>83</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>86</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="92">
                   <c:v>99</c:v>
                 </c:pt>
               </c:numCache>
@@ -448,288 +406,243 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'micro-benchmark'!$B$6:$B$98</c:f>
+              <c:f>'micro-benchmark'!$B$6:$B$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="93"/>
+                <c:ptCount val="78"/>
                 <c:pt idx="0">
-                  <c:v>8425.8121250000004</c:v>
+                  <c:v>9610.821199</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15248.609885</c:v>
+                  <c:v>15645.292143000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20328.718859000001</c:v>
+                  <c:v>21573.592398000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20799.59374</c:v>
+                  <c:v>21276.546246999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26764.435700000002</c:v>
+                  <c:v>27925.288260000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28225.213041999999</c:v>
+                  <c:v>29610.586189000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28721.041406</c:v>
+                  <c:v>29584.938262</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31533.414203</c:v>
+                  <c:v>32324.653081</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>35685.840056000001</c:v>
+                  <c:v>36355.825123000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34826.503639000002</c:v>
+                  <c:v>38384.338823999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>38511.777405000001</c:v>
+                  <c:v>40131.017950000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42844.074767999999</c:v>
+                  <c:v>43233.298418999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>39673.164682000002</c:v>
+                  <c:v>40124.941834999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>38825.395950999999</c:v>
+                  <c:v>42127.348309000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43881.997594</c:v>
+                  <c:v>45370.266831000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>50230.400457000003</c:v>
+                  <c:v>45663.208301999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>44691.117802000001</c:v>
+                  <c:v>51457.833055000003</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>46252.267959999997</c:v>
+                  <c:v>48941.463988000003</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>48454.804716999999</c:v>
+                  <c:v>50180.133332999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>47055.439810000003</c:v>
+                  <c:v>49131.666889</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>49068.101553</c:v>
+                  <c:v>50735.304167000002</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>48594.828120999999</c:v>
+                  <c:v>57242.155525000002</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>57536.261583</c:v>
+                  <c:v>58693.966667000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>53344.087566000002</c:v>
+                  <c:v>53419.937905999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>57203.517011999997</c:v>
+                  <c:v>58226.274900999997</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>52995.717044999998</c:v>
+                  <c:v>52717.733342</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>58707.673951999997</c:v>
+                  <c:v>60286.186106000001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>65239.302467000001</c:v>
+                  <c:v>64383.691887000001</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>58924.458444000004</c:v>
+                  <c:v>60860.453570999998</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>56802.464139999996</c:v>
+                  <c:v>56683.816172999999</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>65758.304671000005</c:v>
+                  <c:v>69157.364877</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>67530.016420999993</c:v>
+                  <c:v>66434.220665000001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>70031.535132000005</c:v>
+                  <c:v>79350.192758000005</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>73173.505799999999</c:v>
+                  <c:v>77514.244166999997</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>68907.503375999993</c:v>
+                  <c:v>81946.788094999996</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>77000.363071999993</c:v>
+                  <c:v>96148</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>65775.046048000004</c:v>
+                  <c:v>80917.5</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>73746.476087000003</c:v>
+                  <c:v>75589.333333000002</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>71147.999165000001</c:v>
+                  <c:v>79577.696190000002</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>74071.311795000001</c:v>
+                  <c:v>79042.772727000003</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>73858.624215000003</c:v>
+                  <c:v>78049.405555999998</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>71199.836957000007</c:v>
+                  <c:v>74561.095237999994</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>74835.012992000004</c:v>
+                  <c:v>79464.764706000002</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>74866.564394000001</c:v>
+                  <c:v>80087.8</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>78922.722678999999</c:v>
+                  <c:v>90401.875</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>80636.047619000004</c:v>
+                  <c:v>91722.527778000003</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>71862.333333000002</c:v>
+                  <c:v>90809.444443999993</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>90425.976250000007</c:v>
+                  <c:v>79612.799383000005</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>88136.271143999998</c:v>
+                  <c:v>86405.978644000003</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>79915.843785000005</c:v>
+                  <c:v>87125.617526000002</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>85169.004979000005</c:v>
+                  <c:v>87854.666666999998</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>79907.228501000005</c:v>
+                  <c:v>86391.455025999996</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>78446.339817999993</c:v>
+                  <c:v>108234.93270799999</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>77156.145457000006</c:v>
+                  <c:v>123595.47195200001</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>105067.73641</c:v>
+                  <c:v>100437.341935</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>118617.765446</c:v>
+                  <c:v>105433.666667</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>95265.618793000001</c:v>
+                  <c:v>79984</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>88218.243589999998</c:v>
+                  <c:v>97860</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>88809.063282999996</c:v>
+                  <c:v>94222.333333000002</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>77844</c:v>
+                  <c:v>117981.17142899999</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>107037.513768</c:v>
+                  <c:v>134361.89333300001</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>99639.921950999997</c:v>
+                  <c:v>106052.333333</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>122582.431111</c:v>
+                  <c:v>114760.91111099999</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>115212.161458</c:v>
+                  <c:v>108071.81</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>114449.450558</c:v>
+                  <c:v>155127.35985400001</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>131343.28888899999</c:v>
+                  <c:v>141090.05079400001</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>126563.162963</c:v>
+                  <c:v>111408.162417</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>101904.8</c:v>
+                  <c:v>145046.1</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>105666.44252900001</c:v>
+                  <c:v>128577.32696599999</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>114952.975869</c:v>
+                  <c:v>119050.88888899999</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>106046.90463999999</c:v>
+                  <c:v>113307.139344</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>156781.010931</c:v>
+                  <c:v>175940</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>127046.529943</c:v>
+                  <c:v>131234.431847</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>115581.05524099999</c:v>
+                  <c:v>126036.333333</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>108972.67834100001</c:v>
+                  <c:v>125221</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>138897.114757</c:v>
+                  <c:v>137986.819048</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>123938.90075299999</c:v>
+                  <c:v>142254.88194699999</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>118282.02426799999</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>115303.337982</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>131001.070378</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>116789.268662</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>118892.778787</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>136592.80737699999</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>134508.88076999999</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>155759.008814</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>149231.8125</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>128122.62397</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>132956.86666699999</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>121712.2</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>125690.281481</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>125158.333333</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>135355.93333299999</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>138536.44452300001</c:v>
+                  <c:v>137390.450476</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -928,147 +841,102 @@
                   <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>47</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>49</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>51</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>52</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>54</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>55</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>56</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>58</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>59</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>60</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>61</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>62</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>63</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>64</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>65</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>66</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>67</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>68</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>69</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>70</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>71</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>73</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>74</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>75</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>76</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>77</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>78</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>79</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>80</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>81</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>82</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>83</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>86</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="92">
                   <c:v>99</c:v>
                 </c:pt>
               </c:numCache>
@@ -1076,288 +944,243 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'micro-benchmark'!$C$6:$C$98</c:f>
+              <c:f>'micro-benchmark'!$C$6:$C$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="93"/>
+                <c:ptCount val="78"/>
                 <c:pt idx="0">
-                  <c:v>2.4025319999999999</c:v>
+                  <c:v>2.7370860000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.296621</c:v>
+                  <c:v>4.4346059999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.7134280000000004</c:v>
+                  <c:v>6.064953</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8394870000000001</c:v>
+                  <c:v>5.9716139999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.4907839999999997</c:v>
+                  <c:v>7.8360900000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.9282880000000002</c:v>
+                  <c:v>8.2838259999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.0398429999999994</c:v>
+                  <c:v>8.2891639999999995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.8039389999999997</c:v>
+                  <c:v>9.0579199999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.9747629999999994</c:v>
+                  <c:v>10.172962999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.7395829999999997</c:v>
+                  <c:v>10.733402</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.762903</c:v>
+                  <c:v>11.242505</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.988196</c:v>
+                  <c:v>12.067821</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11.093190999999999</c:v>
+                  <c:v>11.234565</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10.853907</c:v>
+                  <c:v>11.736606999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12.243377000000001</c:v>
+                  <c:v>12.665385000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>14.046545</c:v>
+                  <c:v>12.736497999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>12.455382</c:v>
+                  <c:v>14.339116000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>12.917083</c:v>
+                  <c:v>13.678433999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>13.523828999999999</c:v>
+                  <c:v>14.02619</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>13.136006999999999</c:v>
+                  <c:v>13.731960000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>13.703919000000001</c:v>
+                  <c:v>14.214582999999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>13.539766999999999</c:v>
+                  <c:v>15.907296000000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>16.050934999999999</c:v>
+                  <c:v>16.421824999999998</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>14.896509999999999</c:v>
+                  <c:v>14.973265</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>15.958318999999999</c:v>
+                  <c:v>16.215129000000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>14.785439999999999</c:v>
+                  <c:v>14.687702</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>16.379593</c:v>
+                  <c:v>16.831965</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>18.194248999999999</c:v>
+                  <c:v>17.921061999999999</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>16.445309999999999</c:v>
+                  <c:v>16.959375000000001</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>15.859073</c:v>
+                  <c:v>15.830598999999999</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>18.332478999999999</c:v>
+                  <c:v>19.283048999999998</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>18.833653000000002</c:v>
+                  <c:v>18.484567999999999</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>19.514942000000001</c:v>
+                  <c:v>22.125843</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>20.417359000000001</c:v>
+                  <c:v>21.640139000000001</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>19.198872999999999</c:v>
+                  <c:v>22.884523999999999</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>21.406652000000001</c:v>
+                  <c:v>26.625</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>18.342587999999999</c:v>
+                  <c:v>22.7</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>20.592390999999999</c:v>
+                  <c:v>20.666667</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>19.802181999999998</c:v>
+                  <c:v>22.139524000000002</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>20.643332999999998</c:v>
+                  <c:v>22.063635999999999</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>20.558105000000001</c:v>
+                  <c:v>21.643056000000001</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>19.918478</c:v>
+                  <c:v>20.702380999999999</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>20.886265000000002</c:v>
+                  <c:v>22.176470999999999</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>20.823864</c:v>
+                  <c:v>22.4</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>22.061159</c:v>
+                  <c:v>25.1875</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>22.357143000000001</c:v>
+                  <c:v>25.555555999999999</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>20</c:v>
+                  <c:v>25.5</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>25.191841</c:v>
+                  <c:v>22.231480999999999</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>24.570896000000001</c:v>
+                  <c:v>24.124441000000001</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>22.238465000000001</c:v>
+                  <c:v>24.297651999999999</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>23.758848</c:v>
+                  <c:v>24.666667</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>22.326815</c:v>
+                  <c:v>24.026454999999999</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>21.834496999999999</c:v>
+                  <c:v>30.13054</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>21.499117999999999</c:v>
+                  <c:v>34.481141999999998</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>29.248459</c:v>
+                  <c:v>27.988261999999999</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>33.013807999999997</c:v>
+                  <c:v>29.25</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>26.530093000000001</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>24.637820999999999</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>24.717981999999999</c:v>
+                  <c:v>26.166667</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>22</c:v>
+                  <c:v>32.774999999999999</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>29.802047999999999</c:v>
+                  <c:v>37.416666999999997</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>27.708537</c:v>
+                  <c:v>29.333333</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>34.148888999999997</c:v>
+                  <c:v>31.966667000000001</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>32.041666999999997</c:v>
+                  <c:v>30.068650999999999</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>31.849651000000001</c:v>
+                  <c:v>43.162706</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>36.549999999999997</c:v>
+                  <c:v>39.268056000000001</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>35.276851999999998</c:v>
+                  <c:v>31.017889</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>28.6</c:v>
+                  <c:v>40.416666999999997</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>29.436782000000001</c:v>
+                  <c:v>35.755605000000003</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>32.003281999999999</c:v>
+                  <c:v>33.333333000000003</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>29.548895000000002</c:v>
+                  <c:v>31.53791</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>43.629297999999999</c:v>
+                  <c:v>48.933332999999998</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>35.364325999999998</c:v>
+                  <c:v>36.558202000000001</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>32.12388</c:v>
+                  <c:v>35.055556000000003</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>30.33379</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>38.622261999999999</c:v>
+                  <c:v>38.385714</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>34.498168999999997</c:v>
+                  <c:v>39.524023999999997</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>32.961972000000003</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>32.077930000000002</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>36.470227000000001</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>32.509653999999998</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>33.099742999999997</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>37.948770000000003</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>37.450785000000003</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>43.357716000000003</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>41.5</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>35.645947999999997</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>37.019047999999998</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>33.799999999999997</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>34.988889</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>34.880000000000003</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>37.700000000000003</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>38.549565999999999</c:v>
+                  <c:v>38.247365000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1450,7 +1273,7 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1498,6 +1321,7 @@
         <c:axId val="1669036480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="180000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1614,6 +1438,7 @@
         <c:axId val="383512719"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="50"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -1714,6 +1539,7 @@
         <c:crossAx val="419996079"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="10"/>
       </c:valAx>
       <c:catAx>
         <c:axId val="419996079"/>
@@ -2665,13 +2491,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF12E9F-467E-BF4B-9C51-CA0AEB6E7F4B}">
-  <dimension ref="A1:H98"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -2724,28 +2553,28 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>112765.37201599999</v>
+        <v>86253.551726999998</v>
       </c>
       <c r="B3">
-        <v>31.434172</v>
+        <v>24.082497</v>
       </c>
       <c r="C3">
-        <v>587473.96721000003</v>
+        <v>235277.166241</v>
       </c>
       <c r="D3">
-        <v>163.262058</v>
+        <v>65.464890999999994</v>
       </c>
       <c r="E3">
-        <v>1117.211233</v>
+        <v>778.82003699999996</v>
       </c>
       <c r="F3">
-        <v>0.37715900000000002</v>
+        <v>0.27799699999999999</v>
       </c>
       <c r="G3">
-        <v>89885.269839999994</v>
+        <v>77891.619193000006</v>
       </c>
       <c r="H3">
-        <v>25.070108999999999</v>
+        <v>21.714133</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -2758,7 +2587,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -2769,10 +2598,10 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <v>8425.8121250000004</v>
+        <v>9610.821199</v>
       </c>
       <c r="C6">
-        <v>2.4025319999999999</v>
+        <v>2.7370860000000001</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -2780,10 +2609,10 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <v>15248.609885</v>
+        <v>15645.292143000001</v>
       </c>
       <c r="C7">
-        <v>4.296621</v>
+        <v>4.4346059999999996</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -2791,10 +2620,10 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>20328.718859000001</v>
+        <v>21573.592398000001</v>
       </c>
       <c r="C8">
-        <v>5.7134280000000004</v>
+        <v>6.064953</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -2802,10 +2631,10 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>20799.59374</v>
+        <v>21276.546246999998</v>
       </c>
       <c r="C9">
-        <v>5.8394870000000001</v>
+        <v>5.9716139999999998</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -2813,10 +2642,10 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <v>26764.435700000002</v>
+        <v>27925.288260000001</v>
       </c>
       <c r="C10">
-        <v>7.4907839999999997</v>
+        <v>7.8360900000000004</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -2824,10 +2653,10 @@
         <v>6</v>
       </c>
       <c r="B11">
-        <v>28225.213041999999</v>
+        <v>29610.586189000001</v>
       </c>
       <c r="C11">
-        <v>7.9282880000000002</v>
+        <v>8.2838259999999995</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -2835,10 +2664,10 @@
         <v>7</v>
       </c>
       <c r="B12">
-        <v>28721.041406</v>
+        <v>29584.938262</v>
       </c>
       <c r="C12">
-        <v>8.0398429999999994</v>
+        <v>8.2891639999999995</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -2846,10 +2675,10 @@
         <v>8</v>
       </c>
       <c r="B13">
-        <v>31533.414203</v>
+        <v>32324.653081</v>
       </c>
       <c r="C13">
-        <v>8.8039389999999997</v>
+        <v>9.0579199999999993</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -2857,10 +2686,10 @@
         <v>9</v>
       </c>
       <c r="B14">
-        <v>35685.840056000001</v>
+        <v>36355.825123000002</v>
       </c>
       <c r="C14">
-        <v>9.9747629999999994</v>
+        <v>10.172962999999999</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -2868,10 +2697,10 @@
         <v>10</v>
       </c>
       <c r="B15">
-        <v>34826.503639000002</v>
+        <v>38384.338823999999</v>
       </c>
       <c r="C15">
-        <v>9.7395829999999997</v>
+        <v>10.733402</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -2879,10 +2708,10 @@
         <v>11</v>
       </c>
       <c r="B16">
-        <v>38511.777405000001</v>
+        <v>40131.017950000001</v>
       </c>
       <c r="C16">
-        <v>10.762903</v>
+        <v>11.242505</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -2890,10 +2719,10 @@
         <v>12</v>
       </c>
       <c r="B17">
-        <v>42844.074767999999</v>
+        <v>43233.298418999999</v>
       </c>
       <c r="C17">
-        <v>11.988196</v>
+        <v>12.067821</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -2901,10 +2730,10 @@
         <v>13</v>
       </c>
       <c r="B18">
-        <v>39673.164682000002</v>
+        <v>40124.941834999998</v>
       </c>
       <c r="C18">
-        <v>11.093190999999999</v>
+        <v>11.234565</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -2912,10 +2741,10 @@
         <v>14</v>
       </c>
       <c r="B19">
-        <v>38825.395950999999</v>
+        <v>42127.348309000001</v>
       </c>
       <c r="C19">
-        <v>10.853907</v>
+        <v>11.736606999999999</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -2923,10 +2752,10 @@
         <v>15</v>
       </c>
       <c r="B20">
-        <v>43881.997594</v>
+        <v>45370.266831000001</v>
       </c>
       <c r="C20">
-        <v>12.243377000000001</v>
+        <v>12.665385000000001</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -2934,10 +2763,10 @@
         <v>16</v>
       </c>
       <c r="B21">
-        <v>50230.400457000003</v>
+        <v>45663.208301999999</v>
       </c>
       <c r="C21">
-        <v>14.046545</v>
+        <v>12.736497999999999</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -2945,10 +2774,10 @@
         <v>17</v>
       </c>
       <c r="B22">
-        <v>44691.117802000001</v>
+        <v>51457.833055000003</v>
       </c>
       <c r="C22">
-        <v>12.455382</v>
+        <v>14.339116000000001</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -2956,10 +2785,10 @@
         <v>18</v>
       </c>
       <c r="B23">
-        <v>46252.267959999997</v>
+        <v>48941.463988000003</v>
       </c>
       <c r="C23">
-        <v>12.917083</v>
+        <v>13.678433999999999</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2967,10 +2796,10 @@
         <v>19</v>
       </c>
       <c r="B24">
-        <v>48454.804716999999</v>
+        <v>50180.133332999998</v>
       </c>
       <c r="C24">
-        <v>13.523828999999999</v>
+        <v>14.02619</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2978,10 +2807,10 @@
         <v>20</v>
       </c>
       <c r="B25">
-        <v>47055.439810000003</v>
+        <v>49131.666889</v>
       </c>
       <c r="C25">
-        <v>13.136006999999999</v>
+        <v>13.731960000000001</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2989,10 +2818,10 @@
         <v>21</v>
       </c>
       <c r="B26">
-        <v>49068.101553</v>
+        <v>50735.304167000002</v>
       </c>
       <c r="C26">
-        <v>13.703919000000001</v>
+        <v>14.214582999999999</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -3000,10 +2829,10 @@
         <v>22</v>
       </c>
       <c r="B27">
-        <v>48594.828120999999</v>
+        <v>57242.155525000002</v>
       </c>
       <c r="C27">
-        <v>13.539766999999999</v>
+        <v>15.907296000000001</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -3011,10 +2840,10 @@
         <v>23</v>
       </c>
       <c r="B28">
-        <v>57536.261583</v>
+        <v>58693.966667000001</v>
       </c>
       <c r="C28">
-        <v>16.050934999999999</v>
+        <v>16.421824999999998</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -3022,10 +2851,10 @@
         <v>24</v>
       </c>
       <c r="B29">
-        <v>53344.087566000002</v>
+        <v>53419.937905999999</v>
       </c>
       <c r="C29">
-        <v>14.896509999999999</v>
+        <v>14.973265</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -3033,10 +2862,10 @@
         <v>25</v>
       </c>
       <c r="B30">
-        <v>57203.517011999997</v>
+        <v>58226.274900999997</v>
       </c>
       <c r="C30">
-        <v>15.958318999999999</v>
+        <v>16.215129000000001</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -3044,10 +2873,10 @@
         <v>26</v>
       </c>
       <c r="B31">
-        <v>52995.717044999998</v>
+        <v>52717.733342</v>
       </c>
       <c r="C31">
-        <v>14.785439999999999</v>
+        <v>14.687702</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -3055,10 +2884,10 @@
         <v>27</v>
       </c>
       <c r="B32">
-        <v>58707.673951999997</v>
+        <v>60286.186106000001</v>
       </c>
       <c r="C32">
-        <v>16.379593</v>
+        <v>16.831965</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -3066,10 +2895,10 @@
         <v>28</v>
       </c>
       <c r="B33">
-        <v>65239.302467000001</v>
+        <v>64383.691887000001</v>
       </c>
       <c r="C33">
-        <v>18.194248999999999</v>
+        <v>17.921061999999999</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -3077,10 +2906,10 @@
         <v>29</v>
       </c>
       <c r="B34">
-        <v>58924.458444000004</v>
+        <v>60860.453570999998</v>
       </c>
       <c r="C34">
-        <v>16.445309999999999</v>
+        <v>16.959375000000001</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -3088,10 +2917,10 @@
         <v>30</v>
       </c>
       <c r="B35">
-        <v>56802.464139999996</v>
+        <v>56683.816172999999</v>
       </c>
       <c r="C35">
-        <v>15.859073</v>
+        <v>15.830598999999999</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -3099,10 +2928,10 @@
         <v>31</v>
       </c>
       <c r="B36">
-        <v>65758.304671000005</v>
+        <v>69157.364877</v>
       </c>
       <c r="C36">
-        <v>18.332478999999999</v>
+        <v>19.283048999999998</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -3110,10 +2939,10 @@
         <v>32</v>
       </c>
       <c r="B37">
-        <v>67530.016420999993</v>
+        <v>66434.220665000001</v>
       </c>
       <c r="C37">
-        <v>18.833653000000002</v>
+        <v>18.484567999999999</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -3121,10 +2950,10 @@
         <v>33</v>
       </c>
       <c r="B38">
-        <v>70031.535132000005</v>
+        <v>79350.192758000005</v>
       </c>
       <c r="C38">
-        <v>19.514942000000001</v>
+        <v>22.125843</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -3132,10 +2961,10 @@
         <v>34</v>
       </c>
       <c r="B39">
-        <v>73173.505799999999</v>
+        <v>77514.244166999997</v>
       </c>
       <c r="C39">
-        <v>20.417359000000001</v>
+        <v>21.640139000000001</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -3143,10 +2972,10 @@
         <v>35</v>
       </c>
       <c r="B40">
-        <v>68907.503375999993</v>
+        <v>81946.788094999996</v>
       </c>
       <c r="C40">
-        <v>19.198872999999999</v>
+        <v>22.884523999999999</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -3154,10 +2983,10 @@
         <v>36</v>
       </c>
       <c r="B41">
-        <v>77000.363071999993</v>
+        <v>96148</v>
       </c>
       <c r="C41">
-        <v>21.406652000000001</v>
+        <v>26.625</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -3165,10 +2994,10 @@
         <v>37</v>
       </c>
       <c r="B42">
-        <v>65775.046048000004</v>
+        <v>80917.5</v>
       </c>
       <c r="C42">
-        <v>18.342587999999999</v>
+        <v>22.7</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -3176,10 +3005,10 @@
         <v>38</v>
       </c>
       <c r="B43">
-        <v>73746.476087000003</v>
+        <v>75589.333333000002</v>
       </c>
       <c r="C43">
-        <v>20.592390999999999</v>
+        <v>20.666667</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -3187,10 +3016,10 @@
         <v>39</v>
       </c>
       <c r="B44">
-        <v>71147.999165000001</v>
+        <v>79577.696190000002</v>
       </c>
       <c r="C44">
-        <v>19.802181999999998</v>
+        <v>22.139524000000002</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -3198,10 +3027,10 @@
         <v>40</v>
       </c>
       <c r="B45">
-        <v>74071.311795000001</v>
+        <v>79042.772727000003</v>
       </c>
       <c r="C45">
-        <v>20.643332999999998</v>
+        <v>22.063635999999999</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -3209,10 +3038,10 @@
         <v>41</v>
       </c>
       <c r="B46">
-        <v>73858.624215000003</v>
+        <v>78049.405555999998</v>
       </c>
       <c r="C46">
-        <v>20.558105000000001</v>
+        <v>21.643056000000001</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -3220,10 +3049,10 @@
         <v>42</v>
       </c>
       <c r="B47">
-        <v>71199.836957000007</v>
+        <v>74561.095237999994</v>
       </c>
       <c r="C47">
-        <v>19.918478</v>
+        <v>20.702380999999999</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -3231,10 +3060,10 @@
         <v>43</v>
       </c>
       <c r="B48">
-        <v>74835.012992000004</v>
+        <v>79464.764706000002</v>
       </c>
       <c r="C48">
-        <v>20.886265000000002</v>
+        <v>22.176470999999999</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -3242,10 +3071,10 @@
         <v>44</v>
       </c>
       <c r="B49">
-        <v>74866.564394000001</v>
+        <v>80087.8</v>
       </c>
       <c r="C49">
-        <v>20.823864</v>
+        <v>22.4</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -3253,538 +3082,373 @@
         <v>45</v>
       </c>
       <c r="B50">
-        <v>78922.722678999999</v>
+        <v>90401.875</v>
       </c>
       <c r="C50">
-        <v>22.061159</v>
+        <v>25.1875</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B51">
-        <v>80636.047619000004</v>
+        <v>91722.527778000003</v>
       </c>
       <c r="C51">
-        <v>22.357143000000001</v>
+        <v>25.555555999999999</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B52">
-        <v>71862.333333000002</v>
+        <v>90809.444443999993</v>
       </c>
       <c r="C52">
-        <v>20</v>
+        <v>25.5</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B53">
-        <v>90425.976250000007</v>
+        <v>79612.799383000005</v>
       </c>
       <c r="C53">
-        <v>25.191841</v>
+        <v>22.231480999999999</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B54">
-        <v>88136.271143999998</v>
+        <v>86405.978644000003</v>
       </c>
       <c r="C54">
-        <v>24.570896000000001</v>
+        <v>24.124441000000001</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B55">
-        <v>79915.843785000005</v>
+        <v>87125.617526000002</v>
       </c>
       <c r="C55">
-        <v>22.238465000000001</v>
+        <v>24.297651999999999</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B56">
-        <v>85169.004979000005</v>
+        <v>87854.666666999998</v>
       </c>
       <c r="C56">
-        <v>23.758848</v>
+        <v>24.666667</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B57">
-        <v>79907.228501000005</v>
+        <v>86391.455025999996</v>
       </c>
       <c r="C57">
-        <v>22.326815</v>
+        <v>24.026454999999999</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B58">
-        <v>78446.339817999993</v>
+        <v>108234.93270799999</v>
       </c>
       <c r="C58">
-        <v>21.834496999999999</v>
+        <v>30.13054</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B59">
-        <v>77156.145457000006</v>
+        <v>123595.47195200001</v>
       </c>
       <c r="C59">
-        <v>21.499117999999999</v>
+        <v>34.481141999999998</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B60">
-        <v>105067.73641</v>
+        <v>100437.341935</v>
       </c>
       <c r="C60">
-        <v>29.248459</v>
+        <v>27.988261999999999</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B61">
-        <v>118617.765446</v>
+        <v>105433.666667</v>
       </c>
       <c r="C61">
-        <v>33.013807999999997</v>
+        <v>29.25</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B62">
-        <v>95265.618793000001</v>
+        <v>79984</v>
       </c>
       <c r="C62">
-        <v>26.530093000000001</v>
+        <v>22</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B63">
-        <v>88218.243589999998</v>
+        <v>97860</v>
       </c>
       <c r="C63">
-        <v>24.637820999999999</v>
+        <v>27</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B64">
-        <v>88809.063282999996</v>
+        <v>94222.333333000002</v>
       </c>
       <c r="C64">
-        <v>24.717981999999999</v>
+        <v>26.166667</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B65">
-        <v>77844</v>
+        <v>117981.17142899999</v>
       </c>
       <c r="C65">
-        <v>22</v>
+        <v>32.774999999999999</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B66">
-        <v>107037.513768</v>
+        <v>134361.89333300001</v>
       </c>
       <c r="C66">
-        <v>29.802047999999999</v>
+        <v>37.416666999999997</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B67">
-        <v>99639.921950999997</v>
+        <v>106052.333333</v>
       </c>
       <c r="C67">
-        <v>27.708537</v>
+        <v>29.333333</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="B68">
-        <v>122582.431111</v>
+        <v>114760.91111099999</v>
       </c>
       <c r="C68">
-        <v>34.148888999999997</v>
+        <v>31.966667000000001</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B69">
-        <v>115212.161458</v>
+        <v>108071.81</v>
       </c>
       <c r="C69">
-        <v>32.041666999999997</v>
+        <v>30.068650999999999</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B70">
-        <v>114449.450558</v>
+        <v>155127.35985400001</v>
       </c>
       <c r="C70">
-        <v>31.849651000000001</v>
+        <v>43.162706</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B71">
-        <v>131343.28888899999</v>
+        <v>141090.05079400001</v>
       </c>
       <c r="C71">
-        <v>36.549999999999997</v>
+        <v>39.268056000000001</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B72">
-        <v>126563.162963</v>
+        <v>111408.162417</v>
       </c>
       <c r="C72">
-        <v>35.276851999999998</v>
+        <v>31.017889</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="B73">
-        <v>101904.8</v>
+        <v>145046.1</v>
       </c>
       <c r="C73">
-        <v>28.6</v>
+        <v>40.416666999999997</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B74">
-        <v>105666.44252900001</v>
+        <v>128577.32696599999</v>
       </c>
       <c r="C74">
-        <v>29.436782000000001</v>
+        <v>35.755605000000003</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B75">
-        <v>114952.975869</v>
+        <v>119050.88888899999</v>
       </c>
       <c r="C75">
-        <v>32.003281999999999</v>
+        <v>33.333333000000003</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="B76">
-        <v>106046.90463999999</v>
+        <v>113307.139344</v>
       </c>
       <c r="C76">
-        <v>29.548895000000002</v>
+        <v>31.53791</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B77">
-        <v>156781.010931</v>
+        <v>175940</v>
       </c>
       <c r="C77">
-        <v>43.629297999999999</v>
+        <v>48.933332999999998</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B78">
-        <v>127046.529943</v>
+        <v>131234.431847</v>
       </c>
       <c r="C78">
-        <v>35.364325999999998</v>
+        <v>36.558202000000001</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B79">
-        <v>115581.05524099999</v>
+        <v>126036.333333</v>
       </c>
       <c r="C79">
-        <v>32.12388</v>
+        <v>35.055556000000003</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B80">
-        <v>108972.67834100001</v>
+        <v>125221</v>
       </c>
       <c r="C80">
-        <v>30.33379</v>
+        <v>35</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B81">
-        <v>138897.114757</v>
+        <v>137986.819048</v>
       </c>
       <c r="C81">
-        <v>38.622261999999999</v>
+        <v>38.385714</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B82">
-        <v>123938.90075299999</v>
+        <v>142254.88194699999</v>
       </c>
       <c r="C82">
-        <v>34.498168999999997</v>
+        <v>39.524023999999997</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="B83">
-        <v>118282.02426799999</v>
+        <v>137390.450476</v>
       </c>
       <c r="C83">
-        <v>32.961972000000003</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84">
-        <v>84</v>
-      </c>
-      <c r="B84">
-        <v>115303.337982</v>
-      </c>
-      <c r="C84">
-        <v>32.077930000000002</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85">
-        <v>85</v>
-      </c>
-      <c r="B85">
-        <v>131001.070378</v>
-      </c>
-      <c r="C85">
-        <v>36.470227000000001</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86">
-        <v>86</v>
-      </c>
-      <c r="B86">
-        <v>116789.268662</v>
-      </c>
-      <c r="C86">
-        <v>32.509653999999998</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87">
-        <v>87</v>
-      </c>
-      <c r="B87">
-        <v>118892.778787</v>
-      </c>
-      <c r="C87">
-        <v>33.099742999999997</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88">
-        <v>88</v>
-      </c>
-      <c r="B88">
-        <v>136592.80737699999</v>
-      </c>
-      <c r="C88">
-        <v>37.948770000000003</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89">
-        <v>89</v>
-      </c>
-      <c r="B89">
-        <v>134508.88076999999</v>
-      </c>
-      <c r="C89">
-        <v>37.450785000000003</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90">
-        <v>90</v>
-      </c>
-      <c r="B90">
-        <v>155759.008814</v>
-      </c>
-      <c r="C90">
-        <v>43.357716000000003</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91">
-        <v>92</v>
-      </c>
-      <c r="B91">
-        <v>149231.8125</v>
-      </c>
-      <c r="C91">
-        <v>41.5</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92">
-        <v>93</v>
-      </c>
-      <c r="B92">
-        <v>128122.62397</v>
-      </c>
-      <c r="C92">
-        <v>35.645947999999997</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93">
-        <v>94</v>
-      </c>
-      <c r="B93">
-        <v>132956.86666699999</v>
-      </c>
-      <c r="C93">
-        <v>37.019047999999998</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94">
-        <v>95</v>
-      </c>
-      <c r="B94">
-        <v>121712.2</v>
-      </c>
-      <c r="C94">
-        <v>33.799999999999997</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95">
-        <v>96</v>
-      </c>
-      <c r="B95">
-        <v>125690.281481</v>
-      </c>
-      <c r="C95">
-        <v>34.988889</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96">
-        <v>97</v>
-      </c>
-      <c r="B96">
-        <v>125158.333333</v>
-      </c>
-      <c r="C96">
-        <v>34.880000000000003</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97">
-        <v>98</v>
-      </c>
-      <c r="B97">
-        <v>135355.93333299999</v>
-      </c>
-      <c r="C97">
-        <v>37.700000000000003</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98">
-        <v>99</v>
-      </c>
-      <c r="B98">
-        <v>138536.44452300001</v>
-      </c>
-      <c r="C98">
-        <v>38.549565999999999</v>
+        <v>38.247365000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>